<commit_message>
easyExcel 读写 excel 文件
</commit_message>
<xml_diff>
--- a/src/test/resources/excelTemplates/客户信息模板.xlsx
+++ b/src/test/resources/excelTemplates/客户信息模板.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wmx\project\IDEA_project\h2Smil\src\test\resources\excelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F72B32-F3F1-433A-8F70-1CC56BB92D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BADB047-BF78-4D49-9EBC-0FF4A90886D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>用户名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -548,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:E8"/>
     </sheetView>
   </sheetViews>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE619CA-58BB-47BA-897A-E978BD6601BD}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>